<commit_message>
Finished adding louisa data processing but need to address multiple images of same well w louisa
</commit_message>
<xml_diff>
--- a/excel_out.xlsx
+++ b/excel_out.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="26">
   <si>
     <t>Area</t>
   </si>
@@ -34,6 +34,9 @@
     <t>Day</t>
   </si>
   <si>
+    <t>210630</t>
+  </si>
+  <si>
     <t>DMSO</t>
   </si>
   <si>
@@ -41,6 +44,9 @@
   </si>
   <si>
     <t>ROCK</t>
+  </si>
+  <si>
+    <t>30uM</t>
   </si>
   <si>
     <t>1</t>
@@ -52,13 +58,25 @@
     <t>5</t>
   </si>
   <si>
+    <t>e5</t>
+  </si>
+  <si>
     <t>01</t>
+  </si>
+  <si>
+    <t>02</t>
   </si>
   <si>
     <t>03</t>
   </si>
   <si>
+    <t>04</t>
+  </si>
+  <si>
     <t>05</t>
+  </si>
+  <si>
+    <t>06</t>
   </si>
   <si>
     <t>07</t>
@@ -74,15 +92,6 @@
   </si>
   <si>
     <t>12</t>
-  </si>
-  <si>
-    <t>02</t>
-  </si>
-  <si>
-    <t>04</t>
-  </si>
-  <si>
-    <t>06</t>
   </si>
 </sst>
 </file>
@@ -440,7 +449,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F73"/>
+  <dimension ref="A1:F240"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -470,360 +479,332 @@
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D2" s="1">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>76671</v>
+        <v>171.78175</v>
       </c>
       <c r="F2">
-        <v>111.6236</v>
+        <v>57.799294</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="C3" s="1"/>
       <c r="D3" s="1">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>42582</v>
+        <v>163.26703</v>
       </c>
       <c r="F3">
-        <v>95.50230400000001</v>
+        <v>52.26354600000001</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>117191</v>
+        <v>1452.3883</v>
       </c>
       <c r="F4">
-        <v>116.38225</v>
+        <v>311.09476</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
-      <c r="C5" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="C5" s="1"/>
       <c r="D5" s="1">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E5">
-        <v>131521</v>
+        <v>52727</v>
       </c>
       <c r="F5">
-        <v>117.10183</v>
+        <v>142.69914</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1">
         <v>14</v>
       </c>
       <c r="E6">
-        <v>184461</v>
+        <v>507.03152</v>
       </c>
       <c r="F6">
-        <v>113.552574</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" s="1">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>55147</v>
+        <v>1153.7395</v>
       </c>
       <c r="F7">
-        <v>78.22561999999999</v>
+        <v>335.3898</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
-      <c r="C8" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="C8" s="1"/>
       <c r="D8" s="1">
         <v>14</v>
       </c>
       <c r="E8">
-        <v>183198</v>
+        <v>326.11984</v>
       </c>
       <c r="F8">
-        <v>110.65667</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9" s="1">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>109524</v>
+        <v>1400.7501</v>
       </c>
       <c r="F9">
-        <v>126.03012</v>
+        <v>514.5</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
-      <c r="C10" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="C10" s="1"/>
       <c r="D10" s="1">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E10">
-        <v>55330</v>
+        <v>121236</v>
       </c>
       <c r="F10">
-        <v>124.613396</v>
+        <v>141.15726</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
       <c r="D11" s="1">
         <v>14</v>
       </c>
       <c r="E11">
-        <v>81980</v>
+        <v>395.41632</v>
       </c>
       <c r="F11">
-        <v>107.9611</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D12" s="1">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>128482</v>
+        <v>1433.1217</v>
       </c>
       <c r="F12">
-        <v>79.04517</v>
+        <v>388.16266</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="C13" s="1"/>
       <c r="D13" s="1">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E13">
-        <v>54584</v>
+        <v>138178</v>
       </c>
       <c r="F13">
-        <v>118.52361</v>
+        <v>157.65814</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D14" s="1">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>43167</v>
+        <v>1296.4636</v>
       </c>
       <c r="F14">
-        <v>95.87798000000001</v>
+        <v>389.24774</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
-      <c r="C15" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="C15" s="1"/>
       <c r="D15" s="1">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E15">
-        <v>34547</v>
+        <v>45654</v>
       </c>
       <c r="F15">
-        <v>106.879555</v>
+        <v>143.5233</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
-      <c r="C16" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="C16" s="1"/>
       <c r="D16" s="1">
         <v>14</v>
       </c>
       <c r="E16">
-        <v>94064</v>
+        <v>598.7422</v>
       </c>
       <c r="F16">
-        <v>108.80487</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D17" s="1">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E17">
-        <v>82192</v>
+        <v>1455.0642</v>
       </c>
       <c r="F17">
-        <v>113.12018</v>
+        <v>407.55167</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
-      <c r="C18" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="C18" s="1"/>
       <c r="D18" s="1">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E18">
-        <v>56554</v>
+        <v>98413</v>
       </c>
       <c r="F18">
-        <v>119.89513</v>
+        <v>150.06352</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D19" s="1">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E19">
-        <v>296687</v>
+        <v>912.5592</v>
       </c>
       <c r="F19">
-        <v>121.98726</v>
+        <v>422.359</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
-      <c r="C20" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="1">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E20">
-        <v>106122</v>
+        <v>107235</v>
       </c>
       <c r="F20">
-        <v>104.84184</v>
+        <v>204.42516</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
-      <c r="C21" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="C21" s="1"/>
       <c r="D21" s="1">
         <v>14</v>
       </c>
       <c r="E21">
-        <v>133591</v>
+        <v>617.9259599999999</v>
       </c>
       <c r="F21">
-        <v>120.24919</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D22" s="1">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E22">
-        <v>67522</v>
+        <v>1803.8086</v>
       </c>
       <c r="F22">
-        <v>82.16843399999999</v>
+        <v>498.66</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1"/>
-      <c r="B23" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
       <c r="D23" s="1">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E23">
-        <v>73034</v>
+        <v>19227</v>
       </c>
       <c r="F23">
-        <v>82.73060600000001</v>
+        <v>196.35732</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -834,200 +815,192 @@
         <v>14</v>
       </c>
       <c r="E24">
-        <v>13992</v>
+        <v>652.3107</v>
       </c>
       <c r="F24">
-        <v>85.10470600000001</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
+      <c r="C25" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="D25" s="1">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E25">
-        <v>20309</v>
+        <v>1598.073</v>
       </c>
       <c r="F25">
-        <v>55.67064</v>
+        <v>378.8357</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
-      <c r="C26" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="C26" s="1"/>
       <c r="D26" s="1">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E26">
-        <v>27634</v>
+        <v>275992</v>
       </c>
       <c r="F26">
-        <v>77.89799000000001</v>
+        <v>159.96812</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
-      <c r="C27" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="C27" s="1"/>
       <c r="D27" s="1">
         <v>14</v>
       </c>
       <c r="E27">
-        <v>104771</v>
+        <v>384.91882</v>
       </c>
       <c r="F27">
-        <v>62.0933</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="D28" s="1">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E28">
-        <v>227672</v>
+        <v>1125.7748</v>
       </c>
       <c r="F28">
-        <v>110.21444</v>
+        <v>494.6826</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
-      <c r="C29" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="C29" s="1"/>
       <c r="D29" s="1">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E29">
-        <v>35242</v>
+        <v>219393</v>
       </c>
       <c r="F29">
-        <v>57.802677</v>
+        <v>178.75366</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
-      <c r="C30" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="C30" s="1"/>
       <c r="D30" s="1">
         <v>14</v>
       </c>
       <c r="E30">
-        <v>69487</v>
+        <v>884.6783</v>
       </c>
       <c r="F30">
-        <v>105.20745</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="D31" s="1">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E31">
-        <v>39264</v>
+        <v>1235.547</v>
       </c>
       <c r="F31">
-        <v>60.333637</v>
+        <v>351.40942</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
-      <c r="C32" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="C32" s="1"/>
       <c r="D32" s="1">
         <v>14</v>
       </c>
       <c r="E32">
-        <v>13595</v>
+        <v>510.8427</v>
       </c>
       <c r="F32">
-        <v>69.81641</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
+      <c r="C33" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="D33" s="1">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E33">
-        <v>126511</v>
+        <v>1699.5112</v>
       </c>
       <c r="F33">
-        <v>109.76343</v>
+        <v>348.0148</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
-      <c r="C34" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="C34" s="1"/>
       <c r="D34" s="1">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E34">
-        <v>74544</v>
+        <v>34870</v>
       </c>
       <c r="F34">
-        <v>93.57983399999999</v>
+        <v>137.4462</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
-      <c r="C35" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="C35" s="1"/>
       <c r="D35" s="1">
         <v>14</v>
       </c>
       <c r="E35">
-        <v>25711</v>
+        <v>362.78888</v>
       </c>
       <c r="F35">
-        <v>63.88643</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="1"/>
+      <c r="A36" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B36" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D36" s="1">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E36">
-        <v>187919</v>
+        <v>1636.3652</v>
       </c>
       <c r="F36">
-        <v>108.57926</v>
+        <v>413.17322</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1035,13 +1008,13 @@
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E37">
-        <v>106299</v>
+        <v>92810</v>
       </c>
       <c r="F37">
-        <v>112.487335</v>
+        <v>131.47256</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1052,24 +1025,26 @@
         <v>14</v>
       </c>
       <c r="E38">
-        <v>390145</v>
+        <v>469.55844</v>
       </c>
       <c r="F38">
-        <v>131.3234</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
+      <c r="C39" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="D39" s="1">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E39">
-        <v>278758</v>
+        <v>1221.5867</v>
       </c>
       <c r="F39">
-        <v>122.395096</v>
+        <v>463.2645</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1077,43 +1052,43 @@
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E40">
-        <v>137123</v>
+        <v>213157</v>
       </c>
       <c r="F40">
-        <v>120.104774</v>
+        <v>182.61058</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
-      <c r="C41" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="C41" s="1"/>
       <c r="D41" s="1">
         <v>14</v>
       </c>
       <c r="E41">
-        <v>428052</v>
+        <v>997.1636</v>
       </c>
       <c r="F41">
-        <v>121.37573</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
+      <c r="C42" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="D42" s="1">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E42">
-        <v>350963</v>
+        <v>1198.1686</v>
       </c>
       <c r="F42">
-        <v>126.754395</v>
+        <v>442.23108</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1121,13 +1096,13 @@
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E43">
-        <v>178537</v>
+        <v>33778</v>
       </c>
       <c r="F43">
-        <v>119.02356</v>
+        <v>130.18228</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1138,272 +1113,246 @@
         <v>14</v>
       </c>
       <c r="E44">
-        <v>191309</v>
+        <v>588.1808</v>
       </c>
       <c r="F44">
-        <v>122.09163</v>
+        <v>45</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D45" s="1">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E45">
-        <v>114473</v>
+        <v>1618.2151</v>
       </c>
       <c r="F45">
-        <v>86.55714</v>
+        <v>418.69968</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
-      <c r="C46" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="C46" s="1"/>
       <c r="D46" s="1">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E46">
-        <v>126330</v>
+        <v>103694</v>
       </c>
       <c r="F46">
-        <v>73.95393</v>
+        <v>163.70628</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
-      <c r="C47" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="C47" s="1"/>
       <c r="D47" s="1">
         <v>14</v>
       </c>
       <c r="E47">
-        <v>109121</v>
+        <v>414.07315</v>
       </c>
       <c r="F47">
-        <v>83.11734</v>
+        <v>41</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D48" s="1">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E48">
-        <v>86009</v>
+        <v>1398.3326</v>
       </c>
       <c r="F48">
-        <v>106.437294</v>
+        <v>424.5388</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
-      <c r="C49" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="C49" s="1"/>
       <c r="D49" s="1">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E49">
-        <v>147223</v>
+        <v>30475</v>
       </c>
       <c r="F49">
-        <v>114.918884</v>
+        <v>121.657196</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
-      <c r="C50" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="C50" s="1"/>
       <c r="D50" s="1">
         <v>14</v>
       </c>
       <c r="E50">
-        <v>166674</v>
+        <v>371.19092</v>
       </c>
       <c r="F50">
-        <v>119.30129</v>
+        <v>50</v>
       </c>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
       <c r="C51" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D51" s="1">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E51">
-        <v>85574</v>
+        <v>1158.6141</v>
       </c>
       <c r="F51">
-        <v>123.15038</v>
+        <v>406.39734</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
-      <c r="C52" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="C52" s="1"/>
       <c r="D52" s="1">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E52">
-        <v>127902</v>
+        <v>88864</v>
       </c>
       <c r="F52">
-        <v>116.08126</v>
+        <v>149.00871</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
-      <c r="C53" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="C53" s="1"/>
       <c r="D53" s="1">
         <v>14</v>
       </c>
       <c r="E53">
-        <v>78160</v>
+        <v>447.16147</v>
       </c>
       <c r="F53">
-        <v>109.68506</v>
+        <v>49</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D54" s="1">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E54">
-        <v>137668</v>
+        <v>1455.3599</v>
       </c>
       <c r="F54">
-        <v>119.43589</v>
+        <v>440.857</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
-      <c r="C55" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="C55" s="1"/>
       <c r="D55" s="1">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E55">
-        <v>144032</v>
+        <v>46269</v>
       </c>
       <c r="F55">
-        <v>118.10176</v>
+        <v>129.69916</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
-      <c r="C56" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="C56" s="1"/>
       <c r="D56" s="1">
         <v>14</v>
       </c>
       <c r="E56">
-        <v>80088</v>
+        <v>519.87213</v>
       </c>
       <c r="F56">
-        <v>122.337425</v>
+        <v>48</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D57" s="1">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E57">
-        <v>32504</v>
+        <v>1557.9543</v>
       </c>
       <c r="F57">
-        <v>109.944466</v>
+        <v>320.86932</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="1"/>
-      <c r="B58" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
       <c r="D58" s="1">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E58">
-        <v>152431</v>
+        <v>24585</v>
       </c>
       <c r="F58">
-        <v>118.07132</v>
+        <v>115.96315</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
-      <c r="C59" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="C59" s="1"/>
       <c r="D59" s="1">
         <v>14</v>
       </c>
       <c r="E59">
-        <v>368437</v>
+        <v>442.78888</v>
       </c>
       <c r="F59">
-        <v>122.47982</v>
+        <v>53</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D60" s="1">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E60">
-        <v>16519</v>
+        <v>1106.3618</v>
       </c>
       <c r="F60">
-        <v>91.587326</v>
+        <v>380.50055</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -1411,45 +1360,43 @@
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E61">
-        <v>51592</v>
+        <v>33252</v>
       </c>
       <c r="F61">
-        <v>75.34794000000001</v>
+        <v>121.34681</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
-      <c r="C62" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="C62" s="1"/>
       <c r="D62" s="1">
         <v>14</v>
       </c>
       <c r="E62">
-        <v>102947</v>
+        <v>904.2468</v>
       </c>
       <c r="F62">
-        <v>115.01536</v>
+        <v>50</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D63" s="1">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E63">
-        <v>12018</v>
+        <v>1041.5466</v>
       </c>
       <c r="F63">
-        <v>79.30254000000001</v>
+        <v>396.43604</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -1457,179 +1404,2709 @@
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E64">
-        <v>62388</v>
+        <v>69092</v>
       </c>
       <c r="F64">
-        <v>76.85715500000001</v>
+        <v>124.02801</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
-      <c r="C65" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="C65" s="1"/>
       <c r="D65" s="1">
         <v>14</v>
       </c>
       <c r="E65">
-        <v>44843</v>
+        <v>647.6661</v>
       </c>
       <c r="F65">
-        <v>102.28914</v>
+        <v>49</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D66" s="1">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E66">
-        <v>85204</v>
+        <v>1746.4706</v>
       </c>
       <c r="F66">
-        <v>108.90031</v>
+        <v>457.75076</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" s="1"/>
-      <c r="B67" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
       <c r="D67" s="1">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E67">
-        <v>44633</v>
+        <v>137335</v>
       </c>
       <c r="F67">
-        <v>100.592026</v>
+        <v>152.99454</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
-      <c r="C68" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="C68" s="1"/>
       <c r="D68" s="1">
         <v>14</v>
       </c>
       <c r="E68">
-        <v>21282</v>
+        <v>794.33514</v>
       </c>
       <c r="F68">
-        <v>101.65614</v>
+        <v>48</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="D69" s="1">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E69">
-        <v>231375</v>
+        <v>1742.8391</v>
       </c>
       <c r="F69">
-        <v>118.90439</v>
+        <v>412.68506</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
-      <c r="C70" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="C70" s="1"/>
       <c r="D70" s="1">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E70">
-        <v>71775</v>
+        <v>14261</v>
       </c>
       <c r="F70">
-        <v>122.64674</v>
+        <v>94.97244000000001</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
-      <c r="C71" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="C71" s="1"/>
       <c r="D71" s="1">
         <v>14</v>
       </c>
       <c r="E71">
-        <v>116160</v>
+        <v>1</v>
       </c>
       <c r="F71">
-        <v>115.458046</v>
+        <v>55</v>
       </c>
     </row>
     <row r="72" spans="1:6">
       <c r="A72" s="1"/>
-      <c r="B72" s="1"/>
+      <c r="B72" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="C72" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D72" s="1">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E72">
-        <v>131433</v>
+        <v>620.3819599999999</v>
       </c>
       <c r="F72">
-        <v>116.497765</v>
+        <v>119.53837</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
-      <c r="C73" s="1" t="s">
+      <c r="C73" s="1"/>
+      <c r="D73" s="1">
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <v>1334.7231</v>
+      </c>
+      <c r="F73">
+        <v>438.2559</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
+      <c r="D74" s="1">
+        <v>7</v>
+      </c>
+      <c r="E74">
+        <v>186044</v>
+      </c>
+      <c r="F74">
+        <v>158.90117</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75" s="1"/>
+      <c r="B75" s="1"/>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1">
+        <v>14</v>
+      </c>
+      <c r="E75">
+        <v>447.8772</v>
+      </c>
+      <c r="F75">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" s="1"/>
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1">
+        <v>14</v>
+      </c>
+      <c r="E76">
+        <v>181.06602</v>
+      </c>
+      <c r="F76">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" s="1"/>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1">
+        <v>14</v>
+      </c>
+      <c r="E77">
+        <v>342.69342</v>
+      </c>
+      <c r="F77">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
+      <c r="C78" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D78" s="1">
+        <v>0</v>
+      </c>
+      <c r="E78">
+        <v>1825.6603</v>
+      </c>
+      <c r="F78">
+        <v>381.8681</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
+      <c r="D79" s="1">
+        <v>7</v>
+      </c>
+      <c r="E79">
+        <v>48155</v>
+      </c>
+      <c r="F79">
+        <v>124.306656</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
+      <c r="C80" s="1"/>
+      <c r="D80" s="1">
+        <v>14</v>
+      </c>
+      <c r="E80">
+        <v>257.4508</v>
+      </c>
+      <c r="F80">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81" s="1"/>
+      <c r="B81" s="1"/>
+      <c r="C81" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D81" s="1">
+        <v>0</v>
+      </c>
+      <c r="E81">
+        <v>1282.8379</v>
+      </c>
+      <c r="F81">
+        <v>407.10855</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" s="1"/>
+      <c r="B82" s="1"/>
+      <c r="C82" s="1"/>
+      <c r="D82" s="1">
+        <v>7</v>
+      </c>
+      <c r="E82">
+        <v>132543</v>
+      </c>
+      <c r="F82">
+        <v>94.6327</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" s="1"/>
+      <c r="B83" s="1"/>
+      <c r="C83" s="1"/>
+      <c r="D83" s="1">
+        <v>14</v>
+      </c>
+      <c r="E83">
+        <v>649.62445</v>
+      </c>
+      <c r="F83">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84" s="1"/>
+      <c r="B84" s="1"/>
+      <c r="C84" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D84" s="1">
+        <v>0</v>
+      </c>
+      <c r="E84">
+        <v>1528.8177</v>
+      </c>
+      <c r="F84">
+        <v>298.45688</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" s="1"/>
+      <c r="B85" s="1"/>
+      <c r="C85" s="1"/>
+      <c r="D85" s="1">
+        <v>7</v>
+      </c>
+      <c r="E85">
+        <v>244791</v>
+      </c>
+      <c r="F85">
+        <v>159.71832</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" s="1"/>
+      <c r="B86" s="1"/>
+      <c r="C86" s="1"/>
+      <c r="D86" s="1">
+        <v>14</v>
+      </c>
+      <c r="E86">
+        <v>827.4012</v>
+      </c>
+      <c r="F86">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" s="1"/>
+      <c r="B87" s="1"/>
+      <c r="C87" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D87" s="1">
+        <v>0</v>
+      </c>
+      <c r="E87">
+        <v>1168.646</v>
+      </c>
+      <c r="F87">
+        <v>289.98495</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" s="1"/>
+      <c r="B88" s="1"/>
+      <c r="C88" s="1"/>
+      <c r="D88" s="1">
+        <v>7</v>
+      </c>
+      <c r="E88">
+        <v>207198</v>
+      </c>
+      <c r="F88">
+        <v>173.8469</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" s="1"/>
+      <c r="B89" s="1"/>
+      <c r="C89" s="1"/>
+      <c r="D89" s="1">
+        <v>14</v>
+      </c>
+      <c r="E89">
+        <v>262.79395</v>
+      </c>
+      <c r="F89">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90" s="1"/>
+      <c r="B90" s="1"/>
+      <c r="C90" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D90" s="1">
+        <v>0</v>
+      </c>
+      <c r="E90">
+        <v>1307.5614</v>
+      </c>
+      <c r="F90">
+        <v>403.25153</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91" s="1"/>
+      <c r="B91" s="1"/>
+      <c r="C91" s="1"/>
+      <c r="D91" s="1">
+        <v>7</v>
+      </c>
+      <c r="E91">
+        <v>44301</v>
+      </c>
+      <c r="F91">
+        <v>142.31108</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92" s="1"/>
+      <c r="B92" s="1"/>
+      <c r="C92" s="1"/>
+      <c r="D92" s="1">
+        <v>14</v>
+      </c>
+      <c r="E92">
+        <v>530.8427</v>
+      </c>
+      <c r="F92">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="A93" s="1"/>
+      <c r="B93" s="1"/>
+      <c r="C93" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D93" s="1">
+        <v>0</v>
+      </c>
+      <c r="E93">
+        <v>993.5555400000001</v>
+      </c>
+      <c r="F93">
+        <v>266.7219</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94" s="1"/>
+      <c r="B94" s="1"/>
+      <c r="C94" s="1"/>
+      <c r="D94" s="1">
+        <v>7</v>
+      </c>
+      <c r="E94">
+        <v>193381</v>
+      </c>
+      <c r="F94">
+        <v>158.08078</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95" s="1"/>
+      <c r="B95" s="1"/>
+      <c r="C95" s="1"/>
+      <c r="D95" s="1">
+        <v>14</v>
+      </c>
+      <c r="E95">
+        <v>277.42136</v>
+      </c>
+      <c r="F95">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
+      <c r="A96" s="1"/>
+      <c r="B96" s="1"/>
+      <c r="C96" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D96" s="1">
+        <v>0</v>
+      </c>
+      <c r="E96">
+        <v>1127.201</v>
+      </c>
+      <c r="F96">
+        <v>395.6842</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
+      <c r="A97" s="1"/>
+      <c r="B97" s="1"/>
+      <c r="C97" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D97" s="1">
+        <v>0</v>
+      </c>
+      <c r="E97">
+        <v>1474.9371</v>
+      </c>
+      <c r="F97">
+        <v>475.5353</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98" s="1"/>
+      <c r="B98" s="1"/>
+      <c r="C98" s="1"/>
+      <c r="D98" s="1">
+        <v>7</v>
+      </c>
+      <c r="E98">
+        <v>69601</v>
+      </c>
+      <c r="F98">
+        <v>92.16587</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
+      <c r="A99" s="1"/>
+      <c r="B99" s="1"/>
+      <c r="C99" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D99" s="1">
+        <v>0</v>
+      </c>
+      <c r="E99">
+        <v>1367.8896</v>
+      </c>
+      <c r="F99">
+        <v>433.56046</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
+      <c r="A100" s="1"/>
+      <c r="B100" s="1"/>
+      <c r="C100" s="1"/>
+      <c r="D100" s="1">
+        <v>7</v>
+      </c>
+      <c r="E100">
+        <v>168282</v>
+      </c>
+      <c r="F100">
+        <v>175.68143</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6">
+      <c r="A101" s="1"/>
+      <c r="B101" s="1"/>
+      <c r="C101" s="1"/>
+      <c r="D101" s="1">
+        <v>14</v>
+      </c>
+      <c r="E101">
+        <v>182.61017</v>
+      </c>
+      <c r="F101">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6">
+      <c r="A102" s="1"/>
+      <c r="B102" s="1"/>
+      <c r="C102" s="1"/>
+      <c r="D102" s="1">
+        <v>14</v>
+      </c>
+      <c r="E102">
+        <v>588.2569</v>
+      </c>
+      <c r="F102">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6">
+      <c r="A103" s="1"/>
+      <c r="B103" s="1"/>
+      <c r="C103" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D103" s="1">
+        <v>0</v>
+      </c>
+      <c r="E103">
+        <v>1591.9385</v>
+      </c>
+      <c r="F103">
+        <v>488.99142</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6">
+      <c r="A104" s="1"/>
+      <c r="B104" s="1"/>
+      <c r="C104" s="1"/>
+      <c r="D104" s="1">
+        <v>7</v>
+      </c>
+      <c r="E104">
+        <v>137474</v>
+      </c>
+      <c r="F104">
+        <v>174.71365</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6">
+      <c r="A105" s="1"/>
+      <c r="B105" s="1"/>
+      <c r="C105" s="1"/>
+      <c r="D105" s="1">
+        <v>14</v>
+      </c>
+      <c r="E105">
+        <v>483.74725</v>
+      </c>
+      <c r="F105">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6">
+      <c r="A106" s="1"/>
+      <c r="B106" s="1"/>
+      <c r="C106" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D106" s="1">
+        <v>0</v>
+      </c>
+      <c r="E106">
+        <v>1760.7963</v>
+      </c>
+      <c r="F106">
+        <v>362.19238</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6">
+      <c r="A107" s="1"/>
+      <c r="B107" s="1"/>
+      <c r="C107" s="1"/>
+      <c r="D107" s="1">
+        <v>7</v>
+      </c>
+      <c r="E107">
+        <v>173689</v>
+      </c>
+      <c r="F107">
+        <v>179.11748</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6">
+      <c r="A108" s="1"/>
+      <c r="B108" s="1"/>
+      <c r="C108" s="1"/>
+      <c r="D108" s="1">
+        <v>14</v>
+      </c>
+      <c r="E108">
+        <v>274.1787</v>
+      </c>
+      <c r="F108">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6">
+      <c r="A109" s="1"/>
+      <c r="B109" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C109" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D73" s="1">
-        <v>14</v>
-      </c>
-      <c r="E73">
-        <v>167056</v>
-      </c>
-      <c r="F73">
-        <v>127.97287</v>
+      <c r="D109" s="1">
+        <v>0</v>
+      </c>
+      <c r="E109">
+        <v>1227.9016</v>
+      </c>
+      <c r="F109">
+        <v>407.47974</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6">
+      <c r="A110" s="1"/>
+      <c r="B110" s="1"/>
+      <c r="C110" s="1"/>
+      <c r="D110" s="1">
+        <v>7</v>
+      </c>
+      <c r="E110">
+        <v>254863</v>
+      </c>
+      <c r="F110">
+        <v>166.69246</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6">
+      <c r="A111" s="1"/>
+      <c r="B111" s="1"/>
+      <c r="C111" s="1"/>
+      <c r="D111" s="1">
+        <v>14</v>
+      </c>
+      <c r="E111">
+        <v>1063.129</v>
+      </c>
+      <c r="F111">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6">
+      <c r="A112" s="1"/>
+      <c r="B112" s="1"/>
+      <c r="C112" s="1"/>
+      <c r="D112" s="1">
+        <v>14</v>
+      </c>
+      <c r="E112">
+        <v>860.127</v>
+      </c>
+      <c r="F112">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6">
+      <c r="A113" s="1"/>
+      <c r="B113" s="1"/>
+      <c r="C113" s="1"/>
+      <c r="D113" s="1">
+        <v>14</v>
+      </c>
+      <c r="E113">
+        <v>605.09753</v>
+      </c>
+      <c r="F113">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6">
+      <c r="A114" s="1"/>
+      <c r="B114" s="1"/>
+      <c r="C114" s="1"/>
+      <c r="D114" s="1">
+        <v>14</v>
+      </c>
+      <c r="E114">
+        <v>1418.3616</v>
+      </c>
+      <c r="F114">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6">
+      <c r="A115" s="1"/>
+      <c r="B115" s="1"/>
+      <c r="C115" s="1"/>
+      <c r="D115" s="1">
+        <v>14</v>
+      </c>
+      <c r="E115">
+        <v>95.12489000000001</v>
+      </c>
+      <c r="F115">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6">
+      <c r="A116" s="1"/>
+      <c r="B116" s="1"/>
+      <c r="C116" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D116" s="1">
+        <v>0</v>
+      </c>
+      <c r="E116">
+        <v>1442.9983</v>
+      </c>
+      <c r="F116">
+        <v>394.01324</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6">
+      <c r="A117" s="1"/>
+      <c r="B117" s="1"/>
+      <c r="C117" s="1"/>
+      <c r="D117" s="1">
+        <v>7</v>
+      </c>
+      <c r="E117">
+        <v>234674</v>
+      </c>
+      <c r="F117">
+        <v>135.99883</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6">
+      <c r="A118" s="1"/>
+      <c r="B118" s="1"/>
+      <c r="C118" s="1"/>
+      <c r="D118" s="1">
+        <v>14</v>
+      </c>
+      <c r="E118">
+        <v>1134.9281</v>
+      </c>
+      <c r="F118">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6">
+      <c r="A119" s="1"/>
+      <c r="B119" s="1"/>
+      <c r="C119" s="1"/>
+      <c r="D119" s="1">
+        <v>14</v>
+      </c>
+      <c r="E119">
+        <v>1545.3616</v>
+      </c>
+      <c r="F119">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6">
+      <c r="A120" s="1"/>
+      <c r="B120" s="1"/>
+      <c r="C120" s="1"/>
+      <c r="D120" s="1">
+        <v>14</v>
+      </c>
+      <c r="E120">
+        <v>885.8204300000001</v>
+      </c>
+      <c r="F120">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6">
+      <c r="A121" s="1"/>
+      <c r="B121" s="1"/>
+      <c r="C121" s="1"/>
+      <c r="D121" s="1">
+        <v>14</v>
+      </c>
+      <c r="E121">
+        <v>753.0386999999999</v>
+      </c>
+      <c r="F121">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6">
+      <c r="A122" s="1"/>
+      <c r="B122" s="1"/>
+      <c r="C122" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D122" s="1">
+        <v>0</v>
+      </c>
+      <c r="E122">
+        <v>1594.9313</v>
+      </c>
+      <c r="F122">
+        <v>405.09494</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6">
+      <c r="A123" s="1"/>
+      <c r="B123" s="1"/>
+      <c r="C123" s="1"/>
+      <c r="D123" s="1">
+        <v>7</v>
+      </c>
+      <c r="E123">
+        <v>108126</v>
+      </c>
+      <c r="F123">
+        <v>147.06387</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6">
+      <c r="A124" s="1"/>
+      <c r="B124" s="1"/>
+      <c r="C124" s="1"/>
+      <c r="D124" s="1">
+        <v>14</v>
+      </c>
+      <c r="E124">
+        <v>1127.2661</v>
+      </c>
+      <c r="F124">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6">
+      <c r="A125" s="1"/>
+      <c r="B125" s="1"/>
+      <c r="C125" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D125" s="1">
+        <v>0</v>
+      </c>
+      <c r="E125">
+        <v>1532.158</v>
+      </c>
+      <c r="F125">
+        <v>352.8695</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6">
+      <c r="A126" s="1"/>
+      <c r="B126" s="1"/>
+      <c r="C126" s="1"/>
+      <c r="D126" s="1">
+        <v>7</v>
+      </c>
+      <c r="E126">
+        <v>97971</v>
+      </c>
+      <c r="F126">
+        <v>147.08635</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6">
+      <c r="A127" s="1"/>
+      <c r="B127" s="1"/>
+      <c r="C127" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D127" s="1">
+        <v>0</v>
+      </c>
+      <c r="E127">
+        <v>1656.1316</v>
+      </c>
+      <c r="F127">
+        <v>313.0443</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6">
+      <c r="A128" s="1"/>
+      <c r="B128" s="1"/>
+      <c r="C128" s="1"/>
+      <c r="D128" s="1">
+        <v>7</v>
+      </c>
+      <c r="E128">
+        <v>304916</v>
+      </c>
+      <c r="F128">
+        <v>149.15746</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6">
+      <c r="A129" s="1"/>
+      <c r="B129" s="1"/>
+      <c r="C129" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D129" s="1">
+        <v>0</v>
+      </c>
+      <c r="E129">
+        <v>1560.8601</v>
+      </c>
+      <c r="F129">
+        <v>289.7989</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6">
+      <c r="A130" s="1"/>
+      <c r="B130" s="1"/>
+      <c r="C130" s="1"/>
+      <c r="D130" s="1">
+        <v>7</v>
+      </c>
+      <c r="E130">
+        <v>289254</v>
+      </c>
+      <c r="F130">
+        <v>145.02838</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6">
+      <c r="A131" s="1"/>
+      <c r="B131" s="1"/>
+      <c r="C131" s="1"/>
+      <c r="D131" s="1">
+        <v>14</v>
+      </c>
+      <c r="E131">
+        <v>769.1442</v>
+      </c>
+      <c r="F131">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6">
+      <c r="A132" s="1"/>
+      <c r="B132" s="1"/>
+      <c r="C132" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D132" s="1">
+        <v>0</v>
+      </c>
+      <c r="E132">
+        <v>1452.3534</v>
+      </c>
+      <c r="F132">
+        <v>467.6563</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6">
+      <c r="A133" s="1"/>
+      <c r="B133" s="1"/>
+      <c r="C133" s="1"/>
+      <c r="D133" s="1">
+        <v>7</v>
+      </c>
+      <c r="E133">
+        <v>289212</v>
+      </c>
+      <c r="F133">
+        <v>154.90886</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6">
+      <c r="A134" s="1"/>
+      <c r="B134" s="1"/>
+      <c r="C134" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D134" s="1">
+        <v>0</v>
+      </c>
+      <c r="E134">
+        <v>1535.9812</v>
+      </c>
+      <c r="F134">
+        <v>333.88184</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6">
+      <c r="A135" s="1"/>
+      <c r="B135" s="1"/>
+      <c r="C135" s="1"/>
+      <c r="D135" s="1">
+        <v>7</v>
+      </c>
+      <c r="E135">
+        <v>79138</v>
+      </c>
+      <c r="F135">
+        <v>116.338165</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6">
+      <c r="A136" s="1"/>
+      <c r="B136" s="1"/>
+      <c r="C136" s="1"/>
+      <c r="D136" s="1">
+        <v>14</v>
+      </c>
+      <c r="E136">
+        <v>523.0436999999999</v>
+      </c>
+      <c r="F136">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6">
+      <c r="A137" s="1"/>
+      <c r="B137" s="1"/>
+      <c r="C137" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D137" s="1">
+        <v>0</v>
+      </c>
+      <c r="E137">
+        <v>1562.5076</v>
+      </c>
+      <c r="F137">
+        <v>310.81805</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6">
+      <c r="A138" s="1"/>
+      <c r="B138" s="1"/>
+      <c r="C138" s="1"/>
+      <c r="D138" s="1">
+        <v>7</v>
+      </c>
+      <c r="E138">
+        <v>84546</v>
+      </c>
+      <c r="F138">
+        <v>159.94348</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6">
+      <c r="A139" s="1"/>
+      <c r="B139" s="1"/>
+      <c r="C139" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D139" s="1">
+        <v>0</v>
+      </c>
+      <c r="E139">
+        <v>1765.0513</v>
+      </c>
+      <c r="F139">
+        <v>381.52393</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6">
+      <c r="A140" s="1"/>
+      <c r="B140" s="1"/>
+      <c r="C140" s="1"/>
+      <c r="D140" s="1">
+        <v>7</v>
+      </c>
+      <c r="E140">
+        <v>60319</v>
+      </c>
+      <c r="F140">
+        <v>138.55045</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6">
+      <c r="A141" s="1"/>
+      <c r="B141" s="1"/>
+      <c r="C141" s="1"/>
+      <c r="D141" s="1">
+        <v>14</v>
+      </c>
+      <c r="E141">
+        <v>515.67114</v>
+      </c>
+      <c r="F141">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6">
+      <c r="A142" s="1"/>
+      <c r="B142" s="1"/>
+      <c r="C142" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D142" s="1">
+        <v>0</v>
+      </c>
+      <c r="E142">
+        <v>1390.9897</v>
+      </c>
+      <c r="F142">
+        <v>361.31625</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6">
+      <c r="A143" s="1"/>
+      <c r="B143" s="1"/>
+      <c r="C143" s="1"/>
+      <c r="D143" s="1">
+        <v>7</v>
+      </c>
+      <c r="E143">
+        <v>51751</v>
+      </c>
+      <c r="F143">
+        <v>125.17443</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6">
+      <c r="A144" s="1"/>
+      <c r="B144" s="1"/>
+      <c r="C144" s="1"/>
+      <c r="D144" s="1">
+        <v>14</v>
+      </c>
+      <c r="E144">
+        <v>736.13416</v>
+      </c>
+      <c r="F144">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6">
+      <c r="A145" s="1"/>
+      <c r="B145" s="1"/>
+      <c r="C145" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D145" s="1">
+        <v>0</v>
+      </c>
+      <c r="E145">
+        <v>1047.3756</v>
+      </c>
+      <c r="F145">
+        <v>260.455</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6">
+      <c r="A146" s="1"/>
+      <c r="B146" s="1"/>
+      <c r="C146" s="1"/>
+      <c r="D146" s="1">
+        <v>7</v>
+      </c>
+      <c r="E146">
+        <v>48087</v>
+      </c>
+      <c r="F146">
+        <v>149.26482</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6">
+      <c r="A147" s="1"/>
+      <c r="B147" s="1"/>
+      <c r="C147" s="1"/>
+      <c r="D147" s="1">
+        <v>14</v>
+      </c>
+      <c r="E147">
+        <v>717.8549</v>
+      </c>
+      <c r="F147">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6">
+      <c r="A148" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D148" s="1">
+        <v>0</v>
+      </c>
+      <c r="E148">
+        <v>1128.462</v>
+      </c>
+      <c r="F148">
+        <v>458.13565</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6">
+      <c r="A149" s="1"/>
+      <c r="B149" s="1"/>
+      <c r="C149" s="1"/>
+      <c r="D149" s="1">
+        <v>7</v>
+      </c>
+      <c r="E149">
+        <v>37306</v>
+      </c>
+      <c r="F149">
+        <v>132.09856</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6">
+      <c r="A150" s="1"/>
+      <c r="B150" s="1"/>
+      <c r="C150" s="1"/>
+      <c r="D150" s="1">
+        <v>14</v>
+      </c>
+      <c r="E150">
+        <v>441.30362</v>
+      </c>
+      <c r="F150">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6">
+      <c r="A151" s="1"/>
+      <c r="B151" s="1"/>
+      <c r="C151" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D151" s="1">
+        <v>0</v>
+      </c>
+      <c r="E151">
+        <v>1213.3027</v>
+      </c>
+      <c r="F151">
+        <v>382.23074</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6">
+      <c r="A152" s="1"/>
+      <c r="B152" s="1"/>
+      <c r="C152" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D152" s="1">
+        <v>0</v>
+      </c>
+      <c r="E152">
+        <v>1180.1112</v>
+      </c>
+      <c r="F152">
+        <v>319.78207</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6">
+      <c r="A153" s="1"/>
+      <c r="B153" s="1"/>
+      <c r="C153" s="1"/>
+      <c r="D153" s="1">
+        <v>7</v>
+      </c>
+      <c r="E153">
+        <v>105294</v>
+      </c>
+      <c r="F153">
+        <v>81.59519</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6">
+      <c r="A154" s="1"/>
+      <c r="B154" s="1"/>
+      <c r="C154" s="1"/>
+      <c r="D154" s="1">
+        <v>7</v>
+      </c>
+      <c r="E154">
+        <v>8894</v>
+      </c>
+      <c r="F154">
+        <v>80.79503000000001</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6">
+      <c r="A155" s="1"/>
+      <c r="B155" s="1"/>
+      <c r="C155" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D155" s="1">
+        <v>0</v>
+      </c>
+      <c r="E155">
+        <v>1360.7777</v>
+      </c>
+      <c r="F155">
+        <v>393.68805</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6">
+      <c r="A156" s="1"/>
+      <c r="B156" s="1"/>
+      <c r="C156" s="1"/>
+      <c r="D156" s="1">
+        <v>7</v>
+      </c>
+      <c r="E156">
+        <v>177528</v>
+      </c>
+      <c r="F156">
+        <v>158.37636</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6">
+      <c r="A157" s="1"/>
+      <c r="B157" s="1"/>
+      <c r="C157" s="1"/>
+      <c r="D157" s="1">
+        <v>14</v>
+      </c>
+      <c r="E157">
+        <v>595.7422</v>
+      </c>
+      <c r="F157">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6">
+      <c r="A158" s="1"/>
+      <c r="B158" s="1"/>
+      <c r="C158" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D158" s="1">
+        <v>0</v>
+      </c>
+      <c r="E158">
+        <v>1177.576</v>
+      </c>
+      <c r="F158">
+        <v>426.1685</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6">
+      <c r="A159" s="1"/>
+      <c r="B159" s="1"/>
+      <c r="C159" s="1"/>
+      <c r="D159" s="1">
+        <v>7</v>
+      </c>
+      <c r="E159">
+        <v>95127</v>
+      </c>
+      <c r="F159">
+        <v>154.5437</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6">
+      <c r="A160" s="1"/>
+      <c r="B160" s="1"/>
+      <c r="C160" s="1"/>
+      <c r="D160" s="1">
+        <v>14</v>
+      </c>
+      <c r="E160">
+        <v>504.49957</v>
+      </c>
+      <c r="F160">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6">
+      <c r="A161" s="1"/>
+      <c r="B161" s="1"/>
+      <c r="C161" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D161" s="1">
+        <v>0</v>
+      </c>
+      <c r="E161">
+        <v>743.7394400000001</v>
+      </c>
+      <c r="F161">
+        <v>478.76645</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6">
+      <c r="A162" s="1"/>
+      <c r="B162" s="1"/>
+      <c r="C162" s="1"/>
+      <c r="D162" s="1">
+        <v>7</v>
+      </c>
+      <c r="E162">
+        <v>81054</v>
+      </c>
+      <c r="F162">
+        <v>147.59378</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6">
+      <c r="A163" s="1"/>
+      <c r="B163" s="1"/>
+      <c r="C163" s="1"/>
+      <c r="D163" s="1">
+        <v>14</v>
+      </c>
+      <c r="E163">
+        <v>647.41125</v>
+      </c>
+      <c r="F163">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6">
+      <c r="A164" s="1"/>
+      <c r="B164" s="1"/>
+      <c r="C164" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D164" s="1">
+        <v>0</v>
+      </c>
+      <c r="E164">
+        <v>1346.8579</v>
+      </c>
+      <c r="F164">
+        <v>389.89893</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6">
+      <c r="A165" s="1"/>
+      <c r="B165" s="1"/>
+      <c r="C165" s="1"/>
+      <c r="D165" s="1">
+        <v>7</v>
+      </c>
+      <c r="E165">
+        <v>112058</v>
+      </c>
+      <c r="F165">
+        <v>148.87895</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6">
+      <c r="A166" s="1"/>
+      <c r="B166" s="1"/>
+      <c r="C166" s="1"/>
+      <c r="D166" s="1">
+        <v>14</v>
+      </c>
+      <c r="E166">
+        <v>591.18585</v>
+      </c>
+      <c r="F166">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6">
+      <c r="A167" s="1"/>
+      <c r="B167" s="1"/>
+      <c r="C167" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D167" s="1">
+        <v>0</v>
+      </c>
+      <c r="E167">
+        <v>999.7954</v>
+      </c>
+      <c r="F167">
+        <v>396.87967</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6">
+      <c r="A168" s="1"/>
+      <c r="B168" s="1"/>
+      <c r="C168" s="1"/>
+      <c r="D168" s="1">
+        <v>7</v>
+      </c>
+      <c r="E168">
+        <v>25315</v>
+      </c>
+      <c r="F168">
+        <v>134.56204</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6">
+      <c r="A169" s="1"/>
+      <c r="B169" s="1"/>
+      <c r="C169" s="1"/>
+      <c r="D169" s="1">
+        <v>14</v>
+      </c>
+      <c r="E169">
+        <v>616.77167</v>
+      </c>
+      <c r="F169">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6">
+      <c r="A170" s="1"/>
+      <c r="B170" s="1"/>
+      <c r="C170" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D170" s="1">
+        <v>0</v>
+      </c>
+      <c r="E170">
+        <v>1227.4474</v>
+      </c>
+      <c r="F170">
+        <v>320.85428</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6">
+      <c r="A171" s="1"/>
+      <c r="B171" s="1"/>
+      <c r="C171" s="1"/>
+      <c r="D171" s="1">
+        <v>7</v>
+      </c>
+      <c r="E171">
+        <v>48017</v>
+      </c>
+      <c r="F171">
+        <v>133.31245</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6">
+      <c r="A172" s="1"/>
+      <c r="B172" s="1"/>
+      <c r="C172" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D172" s="1">
+        <v>0</v>
+      </c>
+      <c r="E172">
+        <v>982.5968</v>
+      </c>
+      <c r="F172">
+        <v>284.3526</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6">
+      <c r="A173" s="1"/>
+      <c r="B173" s="1"/>
+      <c r="C173" s="1"/>
+      <c r="D173" s="1">
+        <v>7</v>
+      </c>
+      <c r="E173">
+        <v>144416</v>
+      </c>
+      <c r="F173">
+        <v>155.86894</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6">
+      <c r="A174" s="1"/>
+      <c r="B174" s="1"/>
+      <c r="C174" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D174" s="1">
+        <v>0</v>
+      </c>
+      <c r="E174">
+        <v>1057.2606</v>
+      </c>
+      <c r="F174">
+        <v>373.83774</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6">
+      <c r="A175" s="1"/>
+      <c r="B175" s="1"/>
+      <c r="C175" s="1"/>
+      <c r="D175" s="1">
+        <v>7</v>
+      </c>
+      <c r="E175">
+        <v>19870</v>
+      </c>
+      <c r="F175">
+        <v>125.55989</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6">
+      <c r="A176" s="1"/>
+      <c r="B176" s="1"/>
+      <c r="C176" s="1"/>
+      <c r="D176" s="1">
+        <v>14</v>
+      </c>
+      <c r="E176">
+        <v>466.65894</v>
+      </c>
+      <c r="F176">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6">
+      <c r="A177" s="1"/>
+      <c r="B177" s="1"/>
+      <c r="C177" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D177" s="1">
+        <v>0</v>
+      </c>
+      <c r="E177">
+        <v>1358.8025</v>
+      </c>
+      <c r="F177">
+        <v>380.89105</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6">
+      <c r="A178" s="1"/>
+      <c r="B178" s="1"/>
+      <c r="C178" s="1"/>
+      <c r="D178" s="1">
+        <v>7</v>
+      </c>
+      <c r="E178">
+        <v>125590</v>
+      </c>
+      <c r="F178">
+        <v>159.02472</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6">
+      <c r="A179" s="1"/>
+      <c r="B179" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D179" s="1">
+        <v>0</v>
+      </c>
+      <c r="E179">
+        <v>1549.6609</v>
+      </c>
+      <c r="F179">
+        <v>358.32706</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6">
+      <c r="A180" s="1"/>
+      <c r="B180" s="1"/>
+      <c r="C180" s="1"/>
+      <c r="D180" s="1">
+        <v>7</v>
+      </c>
+      <c r="E180">
+        <v>151561</v>
+      </c>
+      <c r="F180">
+        <v>133.68562</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6">
+      <c r="A181" s="1"/>
+      <c r="B181" s="1"/>
+      <c r="C181" s="1"/>
+      <c r="D181" s="1">
+        <v>14</v>
+      </c>
+      <c r="E181">
+        <v>854.5899699999999</v>
+      </c>
+      <c r="F181">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6">
+      <c r="A182" s="1"/>
+      <c r="B182" s="1"/>
+      <c r="C182" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D182" s="1">
+        <v>0</v>
+      </c>
+      <c r="E182">
+        <v>1492.8243</v>
+      </c>
+      <c r="F182">
+        <v>480.6721</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6">
+      <c r="A183" s="1"/>
+      <c r="B183" s="1"/>
+      <c r="C183" s="1"/>
+      <c r="D183" s="1">
+        <v>7</v>
+      </c>
+      <c r="E183">
+        <v>35795</v>
+      </c>
+      <c r="F183">
+        <v>138.14175</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6">
+      <c r="A184" s="1"/>
+      <c r="B184" s="1"/>
+      <c r="C184" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D184" s="1">
+        <v>0</v>
+      </c>
+      <c r="E184">
+        <v>1266.9294</v>
+      </c>
+      <c r="F184">
+        <v>350.18262</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6">
+      <c r="A185" s="1"/>
+      <c r="B185" s="1"/>
+      <c r="C185" s="1"/>
+      <c r="D185" s="1">
+        <v>7</v>
+      </c>
+      <c r="E185">
+        <v>93935</v>
+      </c>
+      <c r="F185">
+        <v>77.75891999999999</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6">
+      <c r="A186" s="1"/>
+      <c r="B186" s="1"/>
+      <c r="C186" s="1"/>
+      <c r="D186" s="1">
+        <v>14</v>
+      </c>
+      <c r="E186">
+        <v>1140.5555</v>
+      </c>
+      <c r="F186">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6">
+      <c r="A187" s="1"/>
+      <c r="B187" s="1"/>
+      <c r="C187" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D187" s="1">
+        <v>0</v>
+      </c>
+      <c r="E187">
+        <v>1587.5115</v>
+      </c>
+      <c r="F187">
+        <v>396.65097</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6">
+      <c r="A188" s="1"/>
+      <c r="B188" s="1"/>
+      <c r="C188" s="1"/>
+      <c r="D188" s="1">
+        <v>7</v>
+      </c>
+      <c r="E188">
+        <v>219835</v>
+      </c>
+      <c r="F188">
+        <v>138.3049</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6">
+      <c r="A189" s="1"/>
+      <c r="B189" s="1"/>
+      <c r="C189" s="1"/>
+      <c r="D189" s="1">
+        <v>14</v>
+      </c>
+      <c r="E189">
+        <v>23.142136</v>
+      </c>
+      <c r="F189">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6">
+      <c r="A190" s="1"/>
+      <c r="B190" s="1"/>
+      <c r="C190" s="1"/>
+      <c r="D190" s="1">
+        <v>14</v>
+      </c>
+      <c r="E190">
+        <v>1</v>
+      </c>
+      <c r="F190">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6">
+      <c r="A191" s="1"/>
+      <c r="B191" s="1"/>
+      <c r="C191" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D191" s="1">
+        <v>0</v>
+      </c>
+      <c r="E191">
+        <v>1624.2675</v>
+      </c>
+      <c r="F191">
+        <v>401.59314</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6">
+      <c r="A192" s="1"/>
+      <c r="B192" s="1"/>
+      <c r="C192" s="1"/>
+      <c r="D192" s="1">
+        <v>7</v>
+      </c>
+      <c r="E192">
+        <v>76373</v>
+      </c>
+      <c r="F192">
+        <v>148.38336</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6">
+      <c r="A193" s="1"/>
+      <c r="B193" s="1"/>
+      <c r="C193" s="1"/>
+      <c r="D193" s="1">
+        <v>14</v>
+      </c>
+      <c r="E193">
+        <v>587.8894</v>
+      </c>
+      <c r="F193">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6">
+      <c r="A194" s="1"/>
+      <c r="B194" s="1"/>
+      <c r="C194" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D194" s="1">
+        <v>0</v>
+      </c>
+      <c r="E194">
+        <v>1545.1978</v>
+      </c>
+      <c r="F194">
+        <v>277.96417</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6">
+      <c r="A195" s="1"/>
+      <c r="B195" s="1"/>
+      <c r="C195" s="1"/>
+      <c r="D195" s="1">
+        <v>7</v>
+      </c>
+      <c r="E195">
+        <v>115752</v>
+      </c>
+      <c r="F195">
+        <v>147.4223</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6">
+      <c r="A196" s="1"/>
+      <c r="B196" s="1"/>
+      <c r="C196" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D196" s="1">
+        <v>0</v>
+      </c>
+      <c r="E196">
+        <v>937.4405</v>
+      </c>
+      <c r="F196">
+        <v>475.0031</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6">
+      <c r="A197" s="1"/>
+      <c r="B197" s="1"/>
+      <c r="C197" s="1"/>
+      <c r="D197" s="1">
+        <v>7</v>
+      </c>
+      <c r="E197">
+        <v>172484</v>
+      </c>
+      <c r="F197">
+        <v>161.4056</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6">
+      <c r="A198" s="1"/>
+      <c r="B198" s="1"/>
+      <c r="C198" s="1"/>
+      <c r="D198" s="1">
+        <v>14</v>
+      </c>
+      <c r="E198">
+        <v>255.93608</v>
+      </c>
+      <c r="F198">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6">
+      <c r="A199" s="1"/>
+      <c r="B199" s="1"/>
+      <c r="C199" s="1"/>
+      <c r="D199" s="1">
+        <v>14</v>
+      </c>
+      <c r="E199">
+        <v>18.656855</v>
+      </c>
+      <c r="F199">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6">
+      <c r="A200" s="1"/>
+      <c r="B200" s="1"/>
+      <c r="C200" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D200" s="1">
+        <v>0</v>
+      </c>
+      <c r="E200">
+        <v>749.2391</v>
+      </c>
+      <c r="F200">
+        <v>316.97113</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6">
+      <c r="A201" s="1"/>
+      <c r="B201" s="1"/>
+      <c r="C201" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D201" s="1">
+        <v>0</v>
+      </c>
+      <c r="E201">
+        <v>1491.3138</v>
+      </c>
+      <c r="F201">
+        <v>392.39847</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6">
+      <c r="A202" s="1"/>
+      <c r="B202" s="1"/>
+      <c r="C202" s="1"/>
+      <c r="D202" s="1">
+        <v>7</v>
+      </c>
+      <c r="E202">
+        <v>130547</v>
+      </c>
+      <c r="F202">
+        <v>140.5887</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6">
+      <c r="A203" s="1"/>
+      <c r="B203" s="1"/>
+      <c r="C203" s="1"/>
+      <c r="D203" s="1">
+        <v>14</v>
+      </c>
+      <c r="E203">
+        <v>491.34525</v>
+      </c>
+      <c r="F203">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6">
+      <c r="A204" s="1"/>
+      <c r="B204" s="1"/>
+      <c r="C204" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D204" s="1">
+        <v>0</v>
+      </c>
+      <c r="E204">
+        <v>1052.6372</v>
+      </c>
+      <c r="F204">
+        <v>299.9392</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6">
+      <c r="A205" s="1"/>
+      <c r="B205" s="1"/>
+      <c r="C205" s="1"/>
+      <c r="D205" s="1">
+        <v>7</v>
+      </c>
+      <c r="E205">
+        <v>32799</v>
+      </c>
+      <c r="F205">
+        <v>137.36891</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6">
+      <c r="A206" s="1"/>
+      <c r="B206" s="1"/>
+      <c r="C206" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D206" s="1">
+        <v>0</v>
+      </c>
+      <c r="E206">
+        <v>1637.9985</v>
+      </c>
+      <c r="F206">
+        <v>408.19528</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6">
+      <c r="A207" s="1"/>
+      <c r="B207" s="1"/>
+      <c r="C207" s="1"/>
+      <c r="D207" s="1">
+        <v>7</v>
+      </c>
+      <c r="E207">
+        <v>85882</v>
+      </c>
+      <c r="F207">
+        <v>129.20396</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6">
+      <c r="A208" s="1"/>
+      <c r="B208" s="1"/>
+      <c r="C208" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D208" s="1">
+        <v>0</v>
+      </c>
+      <c r="E208">
+        <v>1647.7604</v>
+      </c>
+      <c r="F208">
+        <v>393.55496</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6">
+      <c r="A209" s="1"/>
+      <c r="B209" s="1"/>
+      <c r="C209" s="1"/>
+      <c r="D209" s="1">
+        <v>7</v>
+      </c>
+      <c r="E209">
+        <v>146735</v>
+      </c>
+      <c r="F209">
+        <v>148.1323</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6">
+      <c r="A210" s="1"/>
+      <c r="B210" s="1"/>
+      <c r="C210" s="1"/>
+      <c r="D210" s="1">
+        <v>14</v>
+      </c>
+      <c r="E210">
+        <v>512.4823</v>
+      </c>
+      <c r="F210">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6">
+      <c r="A211" s="1"/>
+      <c r="B211" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C211" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D211" s="1">
+        <v>0</v>
+      </c>
+      <c r="E211">
+        <v>374.34662</v>
+      </c>
+      <c r="F211">
+        <v>358.84735</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6">
+      <c r="A212" s="1"/>
+      <c r="B212" s="1"/>
+      <c r="C212" s="1"/>
+      <c r="D212" s="1">
+        <v>7</v>
+      </c>
+      <c r="E212">
+        <v>45836</v>
+      </c>
+      <c r="F212">
+        <v>142.94005</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6">
+      <c r="A213" s="1"/>
+      <c r="B213" s="1"/>
+      <c r="C213" s="1"/>
+      <c r="D213" s="1">
+        <v>14</v>
+      </c>
+      <c r="E213">
+        <v>347.4041</v>
+      </c>
+      <c r="F213">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6">
+      <c r="A214" s="1"/>
+      <c r="B214" s="1"/>
+      <c r="C214" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D214" s="1">
+        <v>0</v>
+      </c>
+      <c r="E214">
+        <v>906.7967</v>
+      </c>
+      <c r="F214">
+        <v>352.94086</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6">
+      <c r="A215" s="1"/>
+      <c r="B215" s="1"/>
+      <c r="C215" s="1"/>
+      <c r="D215" s="1">
+        <v>7</v>
+      </c>
+      <c r="E215">
+        <v>13816</v>
+      </c>
+      <c r="F215">
+        <v>115.577156</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6">
+      <c r="A216" s="1"/>
+      <c r="B216" s="1"/>
+      <c r="C216" s="1"/>
+      <c r="D216" s="1">
+        <v>14</v>
+      </c>
+      <c r="E216">
+        <v>268.70563</v>
+      </c>
+      <c r="F216">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6">
+      <c r="A217" s="1"/>
+      <c r="B217" s="1"/>
+      <c r="C217" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D217" s="1">
+        <v>0</v>
+      </c>
+      <c r="E217">
+        <v>1407.6019</v>
+      </c>
+      <c r="F217">
+        <v>342.0048</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6">
+      <c r="A218" s="1"/>
+      <c r="B218" s="1"/>
+      <c r="C218" s="1"/>
+      <c r="D218" s="1">
+        <v>7</v>
+      </c>
+      <c r="E218">
+        <v>216707</v>
+      </c>
+      <c r="F218">
+        <v>132.03773</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6">
+      <c r="A219" s="1"/>
+      <c r="B219" s="1"/>
+      <c r="C219" s="1"/>
+      <c r="D219" s="1">
+        <v>14</v>
+      </c>
+      <c r="E219">
+        <v>903.3768</v>
+      </c>
+      <c r="F219">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6">
+      <c r="A220" s="1"/>
+      <c r="B220" s="1"/>
+      <c r="C220" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D220" s="1">
+        <v>0</v>
+      </c>
+      <c r="E220">
+        <v>892.4684999999999</v>
+      </c>
+      <c r="F220">
+        <v>338.82715</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6">
+      <c r="A221" s="1"/>
+      <c r="B221" s="1"/>
+      <c r="C221" s="1"/>
+      <c r="D221" s="1">
+        <v>7</v>
+      </c>
+      <c r="E221">
+        <v>87079</v>
+      </c>
+      <c r="F221">
+        <v>153.2914</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6">
+      <c r="A222" s="1"/>
+      <c r="B222" s="1"/>
+      <c r="C222" s="1"/>
+      <c r="D222" s="1">
+        <v>14</v>
+      </c>
+      <c r="E222">
+        <v>519.8011</v>
+      </c>
+      <c r="F222">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6">
+      <c r="A223" s="1"/>
+      <c r="B223" s="1"/>
+      <c r="C223" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D223" s="1">
+        <v>0</v>
+      </c>
+      <c r="E223">
+        <v>1458.9778</v>
+      </c>
+      <c r="F223">
+        <v>420.73605</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6">
+      <c r="A224" s="1"/>
+      <c r="B224" s="1"/>
+      <c r="C224" s="1"/>
+      <c r="D224" s="1">
+        <v>7</v>
+      </c>
+      <c r="E224">
+        <v>78867</v>
+      </c>
+      <c r="F224">
+        <v>144.86441</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6">
+      <c r="A225" s="1"/>
+      <c r="B225" s="1"/>
+      <c r="C225" s="1"/>
+      <c r="D225" s="1">
+        <v>14</v>
+      </c>
+      <c r="E225">
+        <v>501.23254</v>
+      </c>
+      <c r="F225">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6">
+      <c r="A226" s="1"/>
+      <c r="B226" s="1"/>
+      <c r="C226" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D226" s="1">
+        <v>0</v>
+      </c>
+      <c r="E226">
+        <v>1581.9983</v>
+      </c>
+      <c r="F226">
+        <v>315.17178</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6">
+      <c r="A227" s="1"/>
+      <c r="B227" s="1"/>
+      <c r="C227" s="1"/>
+      <c r="D227" s="1">
+        <v>7</v>
+      </c>
+      <c r="E227">
+        <v>6927</v>
+      </c>
+      <c r="F227">
+        <v>184.10019</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6">
+      <c r="A228" s="1"/>
+      <c r="B228" s="1"/>
+      <c r="C228" s="1"/>
+      <c r="D228" s="1">
+        <v>7</v>
+      </c>
+      <c r="E228">
+        <v>77530</v>
+      </c>
+      <c r="F228">
+        <v>137.32066</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6">
+      <c r="A229" s="1"/>
+      <c r="B229" s="1"/>
+      <c r="C229" s="1"/>
+      <c r="D229" s="1">
+        <v>14</v>
+      </c>
+      <c r="E229">
+        <v>665.35236</v>
+      </c>
+      <c r="F229">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6">
+      <c r="A230" s="1"/>
+      <c r="B230" s="1"/>
+      <c r="C230" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D230" s="1">
+        <v>0</v>
+      </c>
+      <c r="E230">
+        <v>1255.6788</v>
+      </c>
+      <c r="F230">
+        <v>341.38095</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6">
+      <c r="A231" s="1"/>
+      <c r="B231" s="1"/>
+      <c r="C231" s="1"/>
+      <c r="D231" s="1">
+        <v>7</v>
+      </c>
+      <c r="E231">
+        <v>105763</v>
+      </c>
+      <c r="F231">
+        <v>155.1268</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6">
+      <c r="A232" s="1"/>
+      <c r="B232" s="1"/>
+      <c r="C232" s="1"/>
+      <c r="D232" s="1">
+        <v>14</v>
+      </c>
+      <c r="E232">
+        <v>788.9625</v>
+      </c>
+      <c r="F232">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6">
+      <c r="A233" s="1"/>
+      <c r="B233" s="1"/>
+      <c r="C233" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D233" s="1">
+        <v>0</v>
+      </c>
+      <c r="E233">
+        <v>1712.2565</v>
+      </c>
+      <c r="F233">
+        <v>413.78552</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6">
+      <c r="A234" s="1"/>
+      <c r="B234" s="1"/>
+      <c r="C234" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D234" s="1">
+        <v>0</v>
+      </c>
+      <c r="E234">
+        <v>665.10406</v>
+      </c>
+      <c r="F234">
+        <v>309.49414</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6">
+      <c r="A235" s="1"/>
+      <c r="B235" s="1"/>
+      <c r="C235" s="1"/>
+      <c r="D235" s="1">
+        <v>7</v>
+      </c>
+      <c r="E235">
+        <v>83276</v>
+      </c>
+      <c r="F235">
+        <v>77.04347</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6">
+      <c r="A236" s="1"/>
+      <c r="B236" s="1"/>
+      <c r="C236" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D236" s="1">
+        <v>0</v>
+      </c>
+      <c r="E236">
+        <v>1184.6124</v>
+      </c>
+      <c r="F236">
+        <v>326.06174</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6">
+      <c r="A237" s="1"/>
+      <c r="B237" s="1"/>
+      <c r="C237" s="1"/>
+      <c r="D237" s="1">
+        <v>7</v>
+      </c>
+      <c r="E237">
+        <v>79664</v>
+      </c>
+      <c r="F237">
+        <v>147.98123</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6">
+      <c r="A238" s="1"/>
+      <c r="B238" s="1"/>
+      <c r="C238" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D238" s="1">
+        <v>0</v>
+      </c>
+      <c r="E238">
+        <v>1626.6482</v>
+      </c>
+      <c r="F238">
+        <v>369.10846</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6">
+      <c r="A239" s="1"/>
+      <c r="B239" s="1"/>
+      <c r="C239" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D239" s="1">
+        <v>0</v>
+      </c>
+      <c r="E239">
+        <v>1201.1355</v>
+      </c>
+      <c r="F239">
+        <v>415.05975</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6">
+      <c r="A240" s="1"/>
+      <c r="B240" s="1"/>
+      <c r="C240" s="1"/>
+      <c r="D240" s="1">
+        <v>7</v>
+      </c>
+      <c r="E240">
+        <v>93424</v>
+      </c>
+      <c r="F240">
+        <v>151.01265</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="A11:A50"/>
-    <mergeCell ref="A51:A73"/>
-    <mergeCell ref="B2:B10"/>
-    <mergeCell ref="B11:B22"/>
-    <mergeCell ref="B23:B35"/>
-    <mergeCell ref="B36:B50"/>
-    <mergeCell ref="B51:B57"/>
-    <mergeCell ref="B58:B66"/>
-    <mergeCell ref="B67:B73"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="C36:C40"/>
-    <mergeCell ref="C41:C44"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="C63:C64"/>
+  <mergeCells count="92">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A35"/>
+    <mergeCell ref="A36:A147"/>
+    <mergeCell ref="A148:A240"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B35"/>
+    <mergeCell ref="B36:B71"/>
+    <mergeCell ref="B72:B108"/>
+    <mergeCell ref="B109:B147"/>
+    <mergeCell ref="B148:B178"/>
+    <mergeCell ref="B179:B210"/>
+    <mergeCell ref="B211:B240"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="C25:C27"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="C33:C35"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="C42:C44"/>
+    <mergeCell ref="C45:C47"/>
+    <mergeCell ref="C48:C50"/>
+    <mergeCell ref="C51:C53"/>
+    <mergeCell ref="C54:C56"/>
+    <mergeCell ref="C57:C59"/>
+    <mergeCell ref="C60:C62"/>
+    <mergeCell ref="C63:C65"/>
+    <mergeCell ref="C66:C68"/>
+    <mergeCell ref="C69:C71"/>
+    <mergeCell ref="C72:C77"/>
+    <mergeCell ref="C78:C80"/>
+    <mergeCell ref="C81:C83"/>
+    <mergeCell ref="C84:C86"/>
+    <mergeCell ref="C87:C89"/>
+    <mergeCell ref="C90:C92"/>
+    <mergeCell ref="C93:C95"/>
+    <mergeCell ref="C97:C98"/>
+    <mergeCell ref="C99:C102"/>
+    <mergeCell ref="C103:C105"/>
+    <mergeCell ref="C106:C108"/>
+    <mergeCell ref="C109:C115"/>
+    <mergeCell ref="C116:C121"/>
+    <mergeCell ref="C122:C124"/>
+    <mergeCell ref="C125:C126"/>
+    <mergeCell ref="C127:C128"/>
+    <mergeCell ref="C129:C131"/>
+    <mergeCell ref="C132:C133"/>
+    <mergeCell ref="C134:C136"/>
+    <mergeCell ref="C137:C138"/>
+    <mergeCell ref="C139:C141"/>
+    <mergeCell ref="C142:C144"/>
+    <mergeCell ref="C145:C147"/>
+    <mergeCell ref="C148:C150"/>
+    <mergeCell ref="C152:C154"/>
+    <mergeCell ref="C155:C157"/>
+    <mergeCell ref="C158:C160"/>
+    <mergeCell ref="C161:C163"/>
+    <mergeCell ref="C164:C166"/>
+    <mergeCell ref="C167:C169"/>
+    <mergeCell ref="C170:C171"/>
+    <mergeCell ref="C172:C173"/>
+    <mergeCell ref="C174:C176"/>
+    <mergeCell ref="C177:C178"/>
+    <mergeCell ref="C179:C181"/>
+    <mergeCell ref="C182:C183"/>
+    <mergeCell ref="C184:C186"/>
+    <mergeCell ref="C187:C190"/>
+    <mergeCell ref="C191:C193"/>
+    <mergeCell ref="C194:C195"/>
+    <mergeCell ref="C196:C199"/>
+    <mergeCell ref="C201:C203"/>
+    <mergeCell ref="C204:C205"/>
+    <mergeCell ref="C206:C207"/>
+    <mergeCell ref="C208:C210"/>
+    <mergeCell ref="C211:C213"/>
+    <mergeCell ref="C214:C216"/>
+    <mergeCell ref="C217:C219"/>
+    <mergeCell ref="C220:C222"/>
+    <mergeCell ref="C223:C225"/>
+    <mergeCell ref="C226:C229"/>
+    <mergeCell ref="C230:C232"/>
+    <mergeCell ref="C234:C235"/>
+    <mergeCell ref="C236:C237"/>
+    <mergeCell ref="C239:C240"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>